<commit_message>
Validation Trace added 4 default
</commit_message>
<xml_diff>
--- a/Tests/Docs/trace_tests_table.xlsx
+++ b/Tests/Docs/trace_tests_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1628465_ed_ac_uk/Documents/Year5/PA/CW2/CacheSimulator/Tests/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1182" documentId="11_F25DC773A252ABDACC10489891195DEA5BDE58E6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E0047ED1-9195-4319-B1E1-659404EC9C86}"/>
+  <xr:revisionPtr revIDLastSave="1335" documentId="11_F25DC773A252ABDACC10489891195DEA5BDE58E6" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C229B70E-56D7-4752-BBDC-975D165A5FA7}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="1200" windowWidth="19800" windowHeight="14175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="1305" windowWidth="19800" windowHeight="14175" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="87">
   <si>
     <t>Test Nr</t>
   </si>
@@ -288,13 +288,22 @@
   </si>
   <si>
     <t>P0 W 2048</t>
+  </si>
+  <si>
+    <t>P2 R 2</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +322,12 @@
       <color theme="0"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -353,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -501,6 +516,17 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -661,23 +687,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -687,8 +702,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1429,31 +1465,31 @@
       <c r="G14" s="14"/>
       <c r="H14" s="15"/>
       <c r="I14" s="8">
-        <f>SUM(I4:I13)</f>
+        <f t="shared" ref="I14:O14" si="0">SUM(I4:I13)</f>
         <v>124</v>
       </c>
       <c r="J14" s="8">
-        <f>SUM(J4:J13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="K14" s="9">
-        <f>SUM(K4:K13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="L14" s="10">
-        <f>SUM(L4:L13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M14" s="9">
-        <f>SUM(M4:M13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N14" s="9">
-        <f>SUM(N4:N13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O14" s="10">
-        <f>SUM(O4:O13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -1467,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4869D03-BC3A-42D8-AB4B-EB4229F8F0AE}">
   <dimension ref="B3:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="129" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1563,7 @@
       <c r="B7" s="50">
         <v>0</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="54" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1568,7 +1604,7 @@
       <c r="B8" s="51">
         <v>1</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="55" t="s">
         <v>78</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -1609,7 +1645,7 @@
       <c r="B9" s="51">
         <v>2</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="55" t="s">
         <v>65</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1651,7 +1687,7 @@
       <c r="B10" s="51">
         <v>3</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="55" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1692,7 +1728,7 @@
       <c r="B11" s="51">
         <v>4</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="55" t="s">
         <v>79</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -1734,7 +1770,7 @@
       <c r="B12" s="51">
         <v>5</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="55" t="s">
         <v>80</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -1775,7 +1811,7 @@
       <c r="B13" s="51">
         <v>6</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="55" t="s">
         <v>66</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1816,7 +1852,7 @@
       <c r="B14" s="51">
         <v>7</v>
       </c>
-      <c r="C14" s="64" t="s">
+      <c r="C14" s="55" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
@@ -1848,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="7">
         <v>1</v>
@@ -1858,7 +1894,7 @@
       <c r="B15" s="51">
         <v>8</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="55" t="s">
         <v>81</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -1900,7 +1936,7 @@
       <c r="B16" s="51">
         <v>9</v>
       </c>
-      <c r="C16" s="64" t="s">
+      <c r="C16" s="55" t="s">
         <v>82</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1915,14 +1951,14 @@
       <c r="G16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="51">
-        <v>2</v>
+      <c r="H16" s="65">
+        <v>18</v>
       </c>
       <c r="I16" s="5">
-        <v>1</v>
-      </c>
-      <c r="J16" s="6">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="J16" s="66">
+        <v>1</v>
       </c>
       <c r="K16" s="7">
         <v>0</v>
@@ -1934,17 +1970,17 @@
         <v>0</v>
       </c>
       <c r="N16" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="51">
         <v>10</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="C17" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="52" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="49" t="s">
@@ -1953,172 +1989,402 @@
       <c r="F17" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="51"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="7"/>
+      <c r="G17" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="51">
+        <v>29</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>1</v>
+      </c>
+      <c r="L17" s="5">
+        <v>1</v>
+      </c>
+      <c r="M17" s="6">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="51">
         <v>11</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="60"/>
+      <c r="C18" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="60">
+        <v>2</v>
+      </c>
+      <c r="I18" s="57">
+        <v>1</v>
+      </c>
+      <c r="J18" s="58">
+        <v>0</v>
+      </c>
+      <c r="K18" s="59">
+        <v>0</v>
+      </c>
+      <c r="L18" s="57">
+        <v>0</v>
+      </c>
+      <c r="M18" s="58">
+        <v>0</v>
+      </c>
+      <c r="N18" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="51">
         <v>12</v>
       </c>
-      <c r="C19" s="64"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="60"/>
+      <c r="C19" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="60">
+        <v>2</v>
+      </c>
+      <c r="I19" s="57">
+        <v>1</v>
+      </c>
+      <c r="J19" s="58">
+        <v>0</v>
+      </c>
+      <c r="K19" s="59">
+        <v>0</v>
+      </c>
+      <c r="L19" s="57">
+        <v>0</v>
+      </c>
+      <c r="M19" s="58">
+        <v>0</v>
+      </c>
+      <c r="N19" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="51">
         <v>13</v>
       </c>
-      <c r="C20" s="64"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="60"/>
+      <c r="C20" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="60">
+        <v>29</v>
+      </c>
+      <c r="I20" s="57">
+        <v>0</v>
+      </c>
+      <c r="J20" s="58">
+        <v>0</v>
+      </c>
+      <c r="K20" s="59">
+        <v>1</v>
+      </c>
+      <c r="L20" s="57">
+        <v>0</v>
+      </c>
+      <c r="M20" s="58">
+        <v>0</v>
+      </c>
+      <c r="N20" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="51">
         <v>14</v>
       </c>
-      <c r="C21" s="64"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="60"/>
+      <c r="C21" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="60">
+        <v>19</v>
+      </c>
+      <c r="I21" s="57">
+        <v>0</v>
+      </c>
+      <c r="J21" s="58">
+        <v>1</v>
+      </c>
+      <c r="K21" s="59">
+        <v>0</v>
+      </c>
+      <c r="L21" s="57">
+        <v>0</v>
+      </c>
+      <c r="M21" s="58">
+        <v>0</v>
+      </c>
+      <c r="N21" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="51">
         <v>15</v>
       </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="60"/>
+      <c r="C22" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="60">
+        <f>15+3*2</f>
+        <v>21</v>
+      </c>
+      <c r="I22" s="57">
+        <v>0</v>
+      </c>
+      <c r="J22" s="58">
+        <v>1</v>
+      </c>
+      <c r="K22" s="59">
+        <v>0</v>
+      </c>
+      <c r="L22" s="57">
+        <v>0</v>
+      </c>
+      <c r="M22" s="58">
+        <v>0</v>
+      </c>
+      <c r="N22" s="59">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" s="51">
         <v>16</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="60"/>
+      <c r="C23" s="55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="60">
+        <v>2</v>
+      </c>
+      <c r="I23" s="57">
+        <v>1</v>
+      </c>
+      <c r="J23" s="58">
+        <v>0</v>
+      </c>
+      <c r="K23" s="59">
+        <v>0</v>
+      </c>
+      <c r="L23" s="57">
+        <v>0</v>
+      </c>
+      <c r="M23" s="58">
+        <v>0</v>
+      </c>
+      <c r="N23" s="59">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" s="51">
         <v>17</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="60"/>
+      <c r="C24" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="59" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="60">
+        <f>16+3*1</f>
+        <v>19</v>
+      </c>
+      <c r="I24" s="57">
+        <v>0</v>
+      </c>
+      <c r="J24" s="58">
+        <v>1</v>
+      </c>
+      <c r="K24" s="59">
+        <v>0</v>
+      </c>
+      <c r="L24" s="57">
+        <v>1</v>
+      </c>
+      <c r="M24" s="58">
+        <v>0</v>
+      </c>
+      <c r="N24" s="59">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" s="51">
         <v>18</v>
       </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="57"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="60"/>
+      <c r="C25" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="I25" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="J25" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="K25" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="L25" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="M25" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="N25" s="59" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B26" s="52">
-        <v>19</v>
-      </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
+      <c r="B26" s="61" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
       <c r="G26" s="62"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="62"/>
+      <c r="H26" s="63">
+        <f>SUM(H7:H24)</f>
+        <v>265</v>
+      </c>
+      <c r="I26" s="64">
+        <f>SUM(I7:I24)</f>
+        <v>7</v>
+      </c>
+      <c r="J26" s="63">
+        <f>SUM(J7:J24)</f>
+        <v>8</v>
+      </c>
+      <c r="K26" s="64">
+        <f>SUM(K7:K24)</f>
+        <v>3</v>
+      </c>
+      <c r="L26" s="63">
+        <f>SUM(L7:L24)</f>
+        <v>2</v>
+      </c>
+      <c r="M26" s="64">
+        <f>SUM(M7:M24)</f>
+        <v>1</v>
+      </c>
+      <c r="N26" s="63">
+        <f>SUM(N7:N24)</f>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>